<commit_message>
removal of uneeded screenshots in excel data
</commit_message>
<xml_diff>
--- a/10 - Spike - Tactical Analysis with PlanetWars/data for spike 10.xlsx
+++ b/10 - Spike - Tactical Analysis with PlanetWars/data for spike 10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benho\Documents\Uni-Work\COS30002-103024841\10 - Spike - Tactical Analysis with PlanetWars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DC7673-3D6A-4C05-B44F-5B6B02E3E8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441ED69C-C66B-483D-87D7-9CD480BFA364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D8D9DE00-6C44-4236-BB00-F51DA115B556}"/>
   </bookViews>
@@ -1415,62 +1415,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>185736</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>77487</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>96302</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF4775BB-5B56-D417-376C-DFDA9CC32143}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1428750" y="942975"/>
-          <a:ext cx="9221487" cy="7535327"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>423861</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1489,54 +1445,10 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>906524</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114343</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{174BFB5F-AB58-7419-0A11-3F815D87B396}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4543425" y="5715000"/>
-          <a:ext cx="11812649" cy="304843"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1862,7 +1774,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,6 +1945,9 @@
       <c r="Y3">
         <v>4</v>
       </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2109,6 +2024,9 @@
       </c>
       <c r="Y4">
         <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>